<commit_message>
Change notes for IDs to remove mentioning
</commit_message>
<xml_diff>
--- a/submission_pack/EGA_submission.xlsx
+++ b/submission_pack/EGA_submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl/work/ega-submissions/submission_pack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266A137B-1990-3A4A-BC7A-A8F143B6CE9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB52D281-1142-9545-965A-321BAE3DDF47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38980" yWindow="460" windowWidth="28140" windowHeight="20900" xr2:uid="{B97D998F-FDD8-5440-ACAC-8270B7EF3683}"/>
+    <workbookView xWindow="38980" yWindow="460" windowWidth="28140" windowHeight="20900" firstSheet="7" activeTab="17" xr2:uid="{B97D998F-FDD8-5440-ACAC-8270B7EF3683}"/>
   </bookViews>
   <sheets>
     <sheet name="Please Read First" sheetId="26" r:id="rId1"/>
@@ -94,7 +94,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{A7D654DF-E286-8D4E-906C-888C0BE5B7B1}" name="library_selection_sorted" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/zl/work/ega-submissions/submission_pack/library_selection_sorted.csv">
+    <textPr sourceFile="/Users/zl/work/ega-submissions/submission_pack/library_selection_sorted.csv">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -102,7 +102,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{FC311B29-6E54-E844-8C56-061E6277C46F}" name="library_source_sorted" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/zl/work/ega-submissions/submission_pack/library_source_sorted.csv">
+    <textPr sourceFile="/Users/zl/work/ega-submissions/submission_pack/library_source_sorted.csv">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -110,7 +110,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{1493E41F-0DD5-7B44-9E08-FFB373F778DD}" name="library_strategy_sorted" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/zl/work/ega-submissions/submission_pack/library_strategy_sorted.csv">
+    <textPr sourceFile="/Users/zl/work/ega-submissions/submission_pack/library_strategy_sorted.csv">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -118,7 +118,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{B6FEBB90-87D3-B34D-83E8-297DBE69A996}" name="run_file_type_sorted" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/zl/work/ega-submissions/submission_pack/run_file_type_sorted.csv">
+    <textPr sourceFile="/Users/zl/work/ega-submissions/submission_pack/run_file_type_sorted.csv">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -1508,9 +1508,6 @@
     <t>The Run_ID or Analysis_ID this file is associated with</t>
   </si>
   <si>
-    <t>The unique accession for this study.</t>
-  </si>
-  <si>
     <t>The alias for this study.</t>
   </si>
   <si>
@@ -1559,9 +1556,6 @@
     <t>Experiment_ID</t>
   </si>
   <si>
-    <t>Unique accession for this experiment.</t>
-  </si>
-  <si>
     <t>Spot_length</t>
   </si>
   <si>
@@ -1700,9 +1694,6 @@
     <t>Run_ID</t>
   </si>
   <si>
-    <t>The unique accession for this run.</t>
-  </si>
-  <si>
     <t>Run_alias</t>
   </si>
   <si>
@@ -1739,9 +1730,6 @@
     <t>If applicable, the name of the contract sequecing center that executed the run.</t>
   </si>
   <si>
-    <t>The unique accession for this dataset.</t>
-  </si>
-  <si>
     <t>Dataset_alias</t>
   </si>
   <si>
@@ -1854,6 +1842,18 @@
   </si>
   <si>
     <t>Each file should be linked to the 'Analysis' worksheet or "Run" worksheet.</t>
+  </si>
+  <si>
+    <t>The unique identifier for this study.</t>
+  </si>
+  <si>
+    <t>The unique identifier for this dataset.</t>
+  </si>
+  <si>
+    <t>Unique identifier for this experiment.</t>
+  </si>
+  <si>
+    <t>The unique identifier for this run.</t>
   </si>
 </sst>
 </file>
@@ -2095,13 +2095,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2109,9 +2102,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2124,6 +2114,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2465,7 +2465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7920B2C-36A2-B44E-837A-50FA98CFB76B}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
@@ -2476,58 +2476,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="30"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="30"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="30"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="14" t="s">
-        <v>535</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="32" t="s">
+        <v>531</v>
+      </c>
+      <c r="B11" s="33"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="9" t="s">
@@ -2542,15 +2542,15 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>532</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2558,23 +2558,23 @@
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2582,15 +2582,15 @@
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2598,26 +2598,26 @@
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="30"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="30"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="13"/>
+      <c r="B23" s="30"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="11"/>
@@ -2635,12 +2635,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
@@ -2650,6 +2644,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2660,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EC84C6-B204-BA4C-A5E6-7F2EF036660A}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2686,10 +2686,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>443</v>
+        <v>540</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2697,10 +2697,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2786,90 +2786,90 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>439</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>440</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>444</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>445</v>
+        <v>442</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>448</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>452</v>
+        <v>446</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>449</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>453</v>
+        <v>447</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="35" t="s">
-        <v>477</v>
+      <c r="B20" s="27" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>474</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>476</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>479</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>480</v>
+        <v>477</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>212</v>
       </c>
-      <c r="B23" s="35" t="s">
-        <v>481</v>
+      <c r="B23" s="27" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>482</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>483</v>
+        <v>480</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2944,10 +2944,10 @@
   <sheetData>
     <row r="2" spans="1:23">
       <c r="A2" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>71</v>
@@ -2980,37 +2980,37 @@
         <v>375</v>
       </c>
       <c r="M2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N2" t="s">
+        <v>442</v>
+      </c>
+      <c r="O2" t="s">
         <v>444</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q2" t="s">
         <v>446</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>447</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>448</v>
-      </c>
-      <c r="R2" t="s">
-        <v>449</v>
       </c>
       <c r="S2" t="s">
         <v>8</v>
       </c>
       <c r="T2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="U2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="V2" t="s">
         <v>212</v>
       </c>
       <c r="W2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -3648,90 +3648,90 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="34">
       <c r="A91" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="B91" s="36" t="s">
-        <v>467</v>
+        <v>455</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -3747,7 +3747,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3770,18 +3770,18 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B2" t="s">
-        <v>490</v>
+        <v>541</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3789,47 +3789,47 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B6" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B7" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B8" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B9" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -3878,28 +3878,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="G1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="H1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -3937,7 +3937,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3945,7 +3945,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3963,7 +3963,7 @@
         <v>69</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -4238,7 +4238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85792D68-D418-C748-8F64-73FBA35DD965}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4647,7 +4647,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4670,37 +4670,37 @@
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>426</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>427</v>
-      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="17" t="s">
         <v>216</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="17" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="8"/>
@@ -4711,10 +4711,10 @@
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="17" t="s">
         <v>111</v>
       </c>
       <c r="C6" s="8"/>
@@ -4725,10 +4725,10 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="17" t="s">
         <v>107</v>
       </c>
       <c r="C7" s="8"/>
@@ -4739,10 +4739,10 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="17" t="s">
         <v>194</v>
       </c>
       <c r="C8" s="8"/>
@@ -4753,10 +4753,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>114</v>
       </c>
       <c r="C9" s="8"/>
@@ -4767,7 +4767,7 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="15" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -4780,7 +4780,7 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="15" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -4793,7 +4793,7 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="15" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -4806,10 +4806,10 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="17" t="s">
         <v>196</v>
       </c>
       <c r="C13" s="8"/>
@@ -4820,10 +4820,10 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="17" t="s">
         <v>195</v>
       </c>
       <c r="C14" s="8"/>
@@ -4834,11 +4834,11 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>428</v>
+      <c r="B15" s="17" t="s">
+        <v>427</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -4848,10 +4848,10 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="17" t="s">
         <v>197</v>
       </c>
       <c r="C16" s="8"/>
@@ -4862,10 +4862,10 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="17" t="s">
         <v>198</v>
       </c>
       <c r="C17" s="8"/>
@@ -4876,10 +4876,10 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="17" t="s">
         <v>199</v>
       </c>
       <c r="C18" s="8"/>
@@ -4888,13 +4888,13 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="20"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>200</v>
       </c>
       <c r="C19" s="8"/>
@@ -4903,24 +4903,24 @@
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="20"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="17" t="s">
         <v>201</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="I20" s="19"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>429</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -4938,300 +4938,300 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="27"/>
-    <col min="2" max="2" width="45" style="27" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="27"/>
-    <col min="4" max="4" width="58.6640625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="15.1640625" style="27"/>
+    <col min="1" max="1" width="15.1640625" style="19"/>
+    <col min="2" max="2" width="45" style="19" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="19"/>
+    <col min="4" max="4" width="58.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="15.1640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="21" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="20" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="29"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="20" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="29"/>
-      <c r="B5" s="28" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="20" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="29"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="20" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="20" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="29"/>
-      <c r="B8" s="28" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="20" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="29"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="20" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="29"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="20" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="29"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="20" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="29"/>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="20" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="34" customFormat="1">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:5" s="26" customFormat="1">
+      <c r="A13" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="24" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="29"/>
-      <c r="B14" s="28" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="20" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="29"/>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="20" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="29"/>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="20" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="29"/>
-      <c r="B17" s="28" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="20" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="20" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="20" t="s">
         <v>187</v>
       </c>
     </row>
@@ -5295,65 +5295,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="T1" s="22" t="s">
-        <v>429</v>
+      <c r="T1" s="17" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -5513,7 +5513,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5536,18 +5536,18 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B2" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5555,7 +5555,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5563,31 +5563,31 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B7" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B8" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -5611,10 +5611,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>71</v>
@@ -5623,13 +5623,13 @@
         <v>73</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="F1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -5652,77 +5652,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="6" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="6" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="6" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="6" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="6" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="6" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="6" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="6" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -5757,25 +5757,25 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -5783,7 +5783,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="12" t="s">
         <v>203</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -5791,31 +5791,31 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="13" t="s">
         <v>380</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="18" t="s">
-        <v>495</v>
+      <c r="A7" s="13" t="s">
+        <v>492</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="12" t="s">
         <v>205</v>
       </c>
       <c r="B9" t="s">
@@ -5827,7 +5827,7 @@
         <v>207</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5856,10 +5856,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5872,10 +5872,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -5902,25 +5902,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="12" t="s">
         <v>205</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -5936,13 +5936,13 @@
         <v>212</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>214</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>